<commit_message>
Bug Fixes - pre-1.0.6, ignoring negative values
</commit_message>
<xml_diff>
--- a/tablaTrazable.xlsx
+++ b/tablaTrazable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisby/Documents/git/lavatorio/codeLav/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF43F88E-EC04-1B49-B2D2-B43D0E37247B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8BEB0E-A8A5-A547-ADCC-8BECC3AA6341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18620" yWindow="14820" windowWidth="28040" windowHeight="17440" xr2:uid="{6ACEEAAC-5881-D846-A111-60303DED86F4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{6ACEEAAC-5881-D846-A111-60303DED86F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>P1-001</t>
   </si>
@@ -54,9 +54,6 @@
     <t>pre-1.0.5</t>
   </si>
   <si>
-    <t>1/17: Reparado microcontrolador, fallo desconocido.</t>
-  </si>
-  <si>
     <t>1/17: Nueva</t>
   </si>
   <si>
@@ -76,6 +73,19 @@
   </si>
   <si>
     <t>Tabla de trazabilidad para HANDWASH CONTROLLER</t>
+  </si>
+  <si>
+    <t>P1-006</t>
+  </si>
+  <si>
+    <t>pre-1.0.6</t>
+  </si>
+  <si>
+    <t>1/17: Reparado microcontrolador, fallo desconocido.
+1/23: Upgraded firmware to pre-1.0.6</t>
+  </si>
+  <si>
+    <t>1/23: Upgraded firmware to pre-1.0.6</t>
   </si>
 </sst>
 </file>
@@ -117,9 +127,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365432AA-3857-4B4A-8994-DF9DC1F070A7}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,27 +461,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -475,10 +489,10 @@
         <v>44136</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -492,7 +506,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -506,7 +520,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -520,7 +534,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -534,7 +548,21 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44520</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
autocycle - pre 1.0.8
</commit_message>
<xml_diff>
--- a/tablaTrazable.xlsx
+++ b/tablaTrazable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisby/Documents/git/lavatorio/codeLav/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8BEB0E-A8A5-A547-ADCC-8BECC3AA6341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67E5059-F828-7A49-9C2E-8EB292949050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{6ACEEAAC-5881-D846-A111-60303DED86F4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{6ACEEAAC-5881-D846-A111-60303DED86F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>P1-001</t>
   </si>
@@ -81,11 +81,27 @@
     <t>pre-1.0.6</t>
   </si>
   <si>
+    <t>1/23: Upgraded firmware to pre-1.0.6</t>
+  </si>
+  <si>
+    <t>P1-007</t>
+  </si>
+  <si>
+    <t>P1-008</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>1/17: Reparado microcontrolador, fallo desconocido.
-1/23: Upgraded firmware to pre-1.0.6</t>
-  </si>
-  <si>
-    <t>1/23: Upgraded firmware to pre-1.0.6</t>
+1/23: Upgraded firmware to pre-1.0.6
+2/6: General check, no problems other than copper areas in mounting holes.</t>
+  </si>
+  <si>
+    <t>2/6: Micro falso? No se pudo programar a la primera.</t>
+  </si>
+  <si>
+    <t>2/6: Ensamble, probada.</t>
   </si>
 </sst>
 </file>
@@ -448,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365432AA-3857-4B4A-8994-DF9DC1F070A7}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,7 +497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -492,7 +508,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -562,7 +578,35 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>38749</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>38749</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added softstart functionality, currently under testing
</commit_message>
<xml_diff>
--- a/tablaTrazable.xlsx
+++ b/tablaTrazable.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisby/Documents/git/lavatorio/codeLav/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67E5059-F828-7A49-9C2E-8EB292949050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB706B99-C5AD-774B-8BFF-D68675CA04F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{6ACEEAAC-5881-D846-A111-60303DED86F4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19360" activeTab="1" xr2:uid="{6ACEEAAC-5881-D846-A111-60303DED86F4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tarjetas" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="87">
   <si>
     <t>P1-001</t>
   </si>
@@ -102,6 +103,201 @@
   </si>
   <si>
     <t>2/6: Ensamble, probada.</t>
+  </si>
+  <si>
+    <t>Ensamble/Subsistema</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Cant. Por ensamble</t>
+  </si>
+  <si>
+    <t>Cant. Por compra</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Precio por compra</t>
+  </si>
+  <si>
+    <t>Precio unidad</t>
+  </si>
+  <si>
+    <t>Precio ensamble</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Imagen/Ref</t>
+  </si>
+  <si>
+    <t>Electrico</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Componentes electronicos</t>
+  </si>
+  <si>
+    <t>Componentes electronicos que conforman la PCB (Linea 1)</t>
+  </si>
+  <si>
+    <t>Fuente 12V</t>
+  </si>
+  <si>
+    <t>Fuente 5V</t>
+  </si>
+  <si>
+    <t>Pantalla</t>
+  </si>
+  <si>
+    <t>Cobertor pantalla</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Montura Sensor</t>
+  </si>
+  <si>
+    <t>Bomba Jabón</t>
+  </si>
+  <si>
+    <t>Valvula jabón</t>
+  </si>
+  <si>
+    <t>Valvula agua</t>
+  </si>
+  <si>
+    <t>Modulo 12V de ebay</t>
+  </si>
+  <si>
+    <t>Modulo 5V de ebay</t>
+  </si>
+  <si>
+    <t>Pantalla SD1106 OLED I2C</t>
+  </si>
+  <si>
+    <t>60cm de cable blindado</t>
+  </si>
+  <si>
+    <t>Conector hermético de 4 pines</t>
+  </si>
+  <si>
+    <t>Pieza impresa en 3D /  Moldeada</t>
+  </si>
+  <si>
+    <t>Trío de diodos de sensor Vishay</t>
+  </si>
+  <si>
+    <t>Conector Pantalla/Sensor</t>
+  </si>
+  <si>
+    <t>Cable Pantalla/Sensor</t>
+  </si>
+  <si>
+    <t>Guía y montura para alinear los diodos e indicador</t>
+  </si>
+  <si>
+    <t>Control retorno de jabon</t>
+  </si>
+  <si>
+    <t>Bomba para impulsar jabon hacia la salida</t>
+  </si>
+  <si>
+    <t>Valvula para control de agua para lavado</t>
+  </si>
+  <si>
+    <t>Termoencogible</t>
+  </si>
+  <si>
+    <t>Soldadura</t>
+  </si>
+  <si>
+    <t>Mano de obra??</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tubo aluminio 9mm</t>
+  </si>
+  <si>
+    <t>Barril de inox</t>
+  </si>
+  <si>
+    <t>Taza de inox</t>
+  </si>
+  <si>
+    <t>Inox para ensamble interno</t>
+  </si>
+  <si>
+    <t>Mecanico</t>
+  </si>
+  <si>
+    <t>Tornillo xx</t>
+  </si>
+  <si>
+    <t>Soldadura para comps electronicos THT</t>
+  </si>
+  <si>
+    <t>Soldadura para comps electronicos PCB SMD</t>
+  </si>
+  <si>
+    <t>Tubería para montura de electronica y salidas de agua/jabon</t>
+  </si>
+  <si>
+    <t>Cilindro de inox</t>
+  </si>
+  <si>
+    <t>Stickers</t>
+  </si>
+  <si>
+    <t>Tapa trasera para alimentación electricidad</t>
+  </si>
+  <si>
+    <t>Caja electronicos</t>
+  </si>
+  <si>
+    <t>Contenedor jabon</t>
+  </si>
+  <si>
+    <t>Superficie para recolección de agua de inox moldeada</t>
+  </si>
+  <si>
+    <t>Caja de protección para la PCB</t>
+  </si>
+  <si>
+    <t>Depósito contenedor de jabón liquído</t>
+  </si>
+  <si>
+    <t>Piezas internas en inox (especificar?)</t>
+  </si>
+  <si>
+    <t>Ensamble bomba jabon en inox</t>
+  </si>
+  <si>
+    <t>Holder bomba jabon</t>
+  </si>
+  <si>
+    <t>Numero de parte</t>
+  </si>
+  <si>
+    <t>especificar todos los tornillos?</t>
+  </si>
+  <si>
+    <t>Stickers (livery/decoracion)</t>
+  </si>
+  <si>
+    <t>Para montaje de switches y entrada de alimentación 110V</t>
+  </si>
+  <si>
+    <t>Tarjeta electronica de control</t>
   </si>
 </sst>
 </file>
@@ -466,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365432AA-3857-4B4A-8994-DF9DC1F070A7}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -613,4 +809,289 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DEB3CA-53E4-5C4F-A4A7-B2B913A1D28A}">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>